<commit_message>
Common: Added some initial data for vendors, atomizers, mods
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/vendors.xlsx
+++ b/upgrade/fixtures/vendors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B841FC73-2528-4EAC-826C-078E65C7352D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA90DB81-CEEA-4A02-94B5-9ADD0A011DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26475" yWindow="4020" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1605" yWindow="4020" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>tab</t>
   </si>
@@ -218,6 +218,21 @@
   </si>
   <si>
     <t>Infamous</t>
+  </si>
+  <si>
+    <t>Acrossvape</t>
+  </si>
+  <si>
+    <t>HussarVape</t>
+  </si>
+  <si>
+    <t>Vicious Ant</t>
+  </si>
+  <si>
+    <t>SvoëMesto</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
 </sst>
 </file>
@@ -591,10 +606,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AEBD79-8DB9-48DF-B83D-337964022B0C}">
-  <dimension ref="A1:A60"/>
+  <dimension ref="A1:A65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,292 +634,317 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A60">
-    <sortCondition ref="A56:A60"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A65">
+    <sortCondition ref="A59:A65"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Common: Added boring stuff for liquid
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/vendors.xlsx
+++ b/upgrade/fixtures/vendors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E191B82B-171C-4A72-B416-6751E27F8585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456B0B9A-A283-47D5-AF71-A0111EBD7962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="7515" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4620" yWindow="1845" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>tab</t>
   </si>
@@ -263,6 +263,24 @@
   </si>
   <si>
     <t>Exvape</t>
+  </si>
+  <si>
+    <t>Tobacco Bastards</t>
+  </si>
+  <si>
+    <t>Rocket Girl</t>
+  </si>
+  <si>
+    <t>Electra</t>
+  </si>
+  <si>
+    <t>Five Pawns</t>
+  </si>
+  <si>
+    <t>MaZa</t>
+  </si>
+  <si>
+    <t>Ripe Vapes</t>
   </si>
 </sst>
 </file>
@@ -636,10 +654,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AEBD79-8DB9-48DF-B83D-337964022B0C}">
-  <dimension ref="A1:A75"/>
+  <dimension ref="A1:A81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,242 +807,272 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A75">
-    <sortCondition ref="A64:A75"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A81">
+    <sortCondition ref="A81"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Common: Fixed upgrades and imports of vendors
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/vendors.xlsx
+++ b/upgrade/fixtures/vendors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marek-hanzal/Projects/github.com/marek-hanzal/puff-smith/upgrade/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456B0B9A-A283-47D5-AF71-A0111EBD7962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1E4826-1F58-5245-9682-2BE0B8D2F37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="1845" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4620" yWindow="1840" windowWidth="23960" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>tab</t>
   </si>
@@ -281,6 +281,15 @@
   </si>
   <si>
     <t>Ripe Vapes</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t>Sony</t>
+  </si>
+  <si>
+    <t>Samsung</t>
   </si>
 </sst>
 </file>
@@ -625,13 +634,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="39.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -639,7 +648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -654,425 +663,440 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AEBD79-8DB9-48DF-B83D-337964022B0C}">
-  <dimension ref="A1:A81"/>
+  <dimension ref="A1:A84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A81">
-    <sortCondition ref="A81"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A84">
+    <sortCondition ref="A62:A84"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>